<commit_message>
draft of w1 slides
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c2-dataviz-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D243E2C-7B01-B14B-954F-CB686396143A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9E9445-ADE1-B149-AD9F-26DBD8DEF60D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21400" yWindow="1480" windowWidth="49940" windowHeight="20220" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>week</t>
   </si>
@@ -75,9 +75,6 @@
     <t>slides</t>
   </si>
   <si>
-    <t>w1p1</t>
-  </si>
-  <si>
     <t>Finals Week</t>
   </si>
   <si>
@@ -253,6 +250,15 @@
   </si>
   <si>
     <t>We cover a lot in this course and so there is some space here to dive deeper into topics we didn't cover thouroughly enough, or additional topics as suggested by you and your peers. Each group will also present on their data visualization portfolios and discuss their journey, including high points and challenges faced along the way.</t>
+  </si>
+  <si>
+    <t>assignments/#draft; homework-2</t>
+  </si>
+  <si>
+    <t>Draft; HW2</t>
+  </si>
+  <si>
+    <t>w1</t>
   </si>
 </sst>
 </file>
@@ -632,8 +638,8 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G2" sqref="G2"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,7 +695,7 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="119" x14ac:dyDescent="0.2">
@@ -700,31 +706,31 @@
         <v>44564</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="153" x14ac:dyDescent="0.2">
@@ -735,26 +741,26 @@
         <v>44571</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -768,10 +774,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>7</v>
@@ -785,32 +791,32 @@
         <v>44585</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -821,32 +827,32 @@
         <v>44592</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="119" x14ac:dyDescent="0.2">
@@ -857,32 +863,32 @@
         <v>44599</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -893,19 +899,19 @@
         <v>44606</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="M8" s="6"/>
     </row>
@@ -917,31 +923,31 @@
         <v>44613</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="M9" s="6"/>
     </row>
@@ -953,26 +959,26 @@
         <v>44620</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -983,10 +989,10 @@
         <v>44627</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -997,17 +1003,17 @@
         <v>44634</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M12" s="6"/>
     </row>

</xml_diff>

<commit_message>
Fix homework link in schedule
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c2-dataviz-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F2B7CB-BD2C-F840-BD4D-B37204D37C68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431172AF-955B-6849-A4C5-52B5CDFA4F85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12020" yWindow="500" windowWidth="33600" windowHeight="19860" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>lab-3</t>
   </si>
   <si>
-    <t>homework-1</t>
-  </si>
-  <si>
     <t>assignments/#proposal</t>
   </si>
   <si>
@@ -280,6 +277,9 @@
   </si>
   <si>
     <t>w6</t>
+  </si>
+  <si>
+    <t>homework</t>
   </si>
 </sst>
 </file>
@@ -658,9 +658,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="185" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="185" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,13 +727,13 @@
         <v>44564</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
@@ -742,13 +742,13 @@
         <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>31</v>
@@ -762,13 +762,13 @@
         <v>44571</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>29</v>
@@ -777,16 +777,16 @@
         <v>7</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -800,7 +800,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>29</v>
@@ -817,13 +817,13 @@
         <v>44585</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>34</v>
@@ -832,22 +832,22 @@
         <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -858,13 +858,13 @@
         <v>44592</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>35</v>
@@ -888,7 +888,7 @@
         <v>20</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="119" x14ac:dyDescent="0.2">
@@ -899,16 +899,16 @@
         <v>44599</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="F7" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>23</v>
@@ -920,13 +920,13 @@
         <v>17</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -937,19 +937,19 @@
         <v>44606</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="M8" s="6"/>
     </row>
@@ -961,10 +961,10 @@
         <v>44613</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>32</v>
@@ -973,19 +973,19 @@
         <v>26</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="J9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="M9" s="6"/>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>32</v>
@@ -1010,13 +1010,13 @@
         <v>26</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -1027,10 +1027,10 @@
         <v>44627</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updating schedule; post recording
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c2-dataviz-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9757AD3F-AB67-5D48-8815-4912E5D35AC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24969600-3E37-3742-8DA7-841C24C9557F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="90">
   <si>
     <t>week</t>
   </si>
@@ -90,9 +90,6 @@
     <t>4; 19</t>
   </si>
   <si>
-    <t>Intro to Geographic data</t>
-  </si>
-  <si>
     <t>lecture_link</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>assignments/#proposal</t>
   </si>
   <si>
-    <t>Building (static) data dashboards with the [{flexdashboard}](https://rmarkdown.rstudio.com/flexdashboard/) package. We'll discuss layouts, including multi-page layouts, storyboards, icons, and publishing through GitHub.</t>
-  </si>
-  <si>
     <t>Visual Perception &amp; Lab 2</t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>Three primary means by which color can aid interpretation. Color blindness considerations and color palettes that work well. Common pitfalls with the use of color. We will use color for each of its primary uses in data visualization and explore and evaluate different palettes by different types of color blindness.</t>
   </si>
   <si>
-    <t>Websites, flex dashbaords, and some customization with CSS</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=X7Cl3lwxXi4; https://www.sds.pub/collaborating-with-git-and-github.html; git-branches.html</t>
   </si>
   <si>
@@ -231,18 +222,9 @@
     <t>7; 15</t>
   </si>
   <si>
-    <t>Understanding the difference between vector and raster data, producing basic maps, getting data for producing different types of maps, and understandin the basics of the R geospatial ecosystem (which is consistently and rapidly evolving).</t>
-  </si>
-  <si>
     <t>We cover a lot in this course and so there is some space here to dive deeper into topics we didn't cover thouroughly enough, or additional topics as suggested by you and your peers. Each group will also present on their data visualization portfolios and discuss their journey, including high points and challenges faced along the way.</t>
   </si>
   <si>
-    <t>assignments/#draft; homework-2</t>
-  </si>
-  <si>
-    <t>Draft; HW2</t>
-  </si>
-  <si>
     <t>w1</t>
   </si>
   <si>
@@ -276,16 +258,43 @@
     <t>Refining your plots for communication. We'll discuss annotating plots, aspect ratios, scales, and a bit on theming.</t>
   </si>
   <si>
-    <t>Common methods for visualizing uncertainty (and their implementation w/{ggplot2}). Framing uncertainty as relative frequencies. Non-standard methods for visualizing standard errors, boostrapping, and a brief foray into hypothetical outcomes plots. We will focus primarily on two packages for creating tables: [{gt}](https://gt.rstudio.com) for static tables, and [{reactable}](https://glin.github.io/reactable/index.html) for interactive tables. We'll also discuss changing fonts, both within websites/applications, as well as with {ggplot2}.</t>
-  </si>
-  <si>
-    <t>Uncertainty &amp; intro to tables and fonts</t>
-  </si>
-  <si>
     <t>https://youtu.be/g1i--4u13bA</t>
   </si>
   <si>
     <t>w7</t>
+  </si>
+  <si>
+    <t>https://youtu.be/uYj04BODzIc</t>
+  </si>
+  <si>
+    <t>Uncertainty</t>
+  </si>
+  <si>
+    <t>Common methods for visualizing uncertainty (and their implementation w/{ggplot2}). Framing uncertainty as relative frequencies. Non-standard methods for visualizing standard errors, boostrapping, and a brief foray into hypothetical outcomes plots. We'll also discuss changing fonts, both within websites/applications, as well as with {ggplot2}.</t>
+  </si>
+  <si>
+    <t>Tables &amp; intro to Geographic data</t>
+  </si>
+  <si>
+    <t>We will focus primarily on two packages for creating tables: [{gt}](https://gt.rstudio.com) for static tables, and [{reactable}](https://glin.github.io/reactable/index.html) for interactive tables. We will also discuss the differences between vector and raster data, producing basic maps, getting data for producing different types of maps, and understandin the basics of the R geospatial ecosystem (which is consistently and rapidly evolving).</t>
+  </si>
+  <si>
+    <t>assignments/#draft</t>
+  </si>
+  <si>
+    <t>assignments/#peer-review; homework-2</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>PR; HW2</t>
+  </si>
+  <si>
+    <t>Websites with [{distill}](https://rstudio.github.io/distill/), which help you create relatively simple yet customizable blogs, optimized for scientific communication. Also building (static) data dashboards with the [{flexdashboard}](https://rmarkdown.rstudio.com/flexdashboard/) package. Finally, we will discuss customization with CSS, and changing the fonts in both web-based documents, as well as ggplot2 plots.</t>
+  </si>
+  <si>
+    <t>Websites, flex dashbaords, fonts, and some customization with CSS</t>
   </si>
 </sst>
 </file>
@@ -664,9 +673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="185" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="185" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,7 +731,7 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="119" x14ac:dyDescent="0.2">
@@ -733,31 +742,31 @@
         <v>44564</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="153" x14ac:dyDescent="0.2">
@@ -768,31 +777,31 @@
         <v>44571</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -806,10 +815,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>7</v>
@@ -823,37 +832,37 @@
         <v>44585</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -864,22 +873,22 @@
         <v>44592</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>8</v>
@@ -894,7 +903,7 @@
         <v>20</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -905,37 +914,37 @@
         <v>44599</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="152" customHeight="1" x14ac:dyDescent="0.2">
@@ -946,26 +955,28 @@
         <v>44606</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -973,35 +984,35 @@
         <v>44613</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1009,26 +1020,26 @@
         <v>44620</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -1039,10 +1050,10 @@
         <v>44627</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1057,13 +1068,13 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M12" s="6"/>
     </row>

</xml_diff>

<commit_message>
post w9 lecture video
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c2-dataviz-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16620F95-2AC0-F946-AC03-31AAF860C225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FA7C06-3D38-6747-B874-2E86AC0288D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
   <si>
     <t>week</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>w8</t>
+  </si>
+  <si>
+    <t>https://youtu.be/1cBa0tqXV6s</t>
   </si>
 </sst>
 </file>
@@ -676,9 +679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="185" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="185" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,7 +1019,9 @@
       <c r="L9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M9" s="6"/>
+      <c r="M9" s="6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="1">

</xml_diff>